<commit_message>
Created Initial Packing Sheet Generator App - Implement Excel to Word converter with drag-and-drop and folder upload support - Add toggleable document preview with centered layout when hidden - Replace generic column numbers with dynamic family names from data headers - Support column splitting with individual documents per family - Include batch download options (separate files and ZIP) - Add transpose functionality for row/column switching - Implement responsive design with Word-like document preview styling
</commit_message>
<xml_diff>
--- a/PackingSheets.xlsx
+++ b/PackingSheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dancikg/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camer\OneDrive\Documents\Desktop\clicktools\CLiCK-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025C9286-8C50-5943-9EBC-4E123D55621C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0563E69-17DE-401F-891F-4DC60E2ECCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="620" windowWidth="28040" windowHeight="15500" xr2:uid="{A19A0EA5-61A4-C64B-839F-4BA47B3201C6}"/>
+    <workbookView xWindow="4620" yWindow="3472" windowWidth="16200" windowHeight="9308" xr2:uid="{A19A0EA5-61A4-C64B-839F-4BA47B3201C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t>Family</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>2 Adults, 3 Children</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Peaches</t>
   </si>
 </sst>
 </file>
@@ -144,9 +150,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -184,7 +190,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -290,7 +296,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -432,7 +438,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -440,23 +446,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCEED3C-565A-9B49-A0F8-18D6F3C43B0D}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.3125" customWidth="1"/>
     <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="22.3125" customWidth="1"/>
+    <col min="5" max="5" width="18.1875" customWidth="1"/>
+    <col min="6" max="6" width="17.8125" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +500,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -529,6 +535,44 @@
         <v>15</v>
       </c>
       <c r="L2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>